<commit_message>
Platform tasarımı ve Spawn işlemleri
Platform ayarlama ve spawn işlemleri
</commit_message>
<xml_diff>
--- a/Zaman Çizelgesi/İş Planı.xlsx
+++ b/Zaman Çizelgesi/İş Planı.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRAGON\Desktop\ymgk\proje\dökümanlar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DRAGON\Documents\GitHub\YMGK_Proje_2\Zaman Çizelgesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Tarih</t>
   </si>
@@ -47,19 +47,10 @@
     <t>Gereksinimlerin Değerlendirilmesi Ve Temel Mekanizmanın Tasarlanması</t>
   </si>
   <si>
-    <t>Giriş Sahnesi  Ve Panellerin Tasarımı</t>
+    <t xml:space="preserve"> Proje hata denetimi ve Proje Teslimi</t>
   </si>
   <si>
-    <t>Oyun Mekanizmasının Yeni Sahneye Uyarlanması</t>
-  </si>
-  <si>
-    <t>Oyun İçin Görsellerin Tasarımı Ve Ses Dosyalarının Eklenmsei</t>
-  </si>
-  <si>
-    <t>Geri Sayım ve Puan Mekanizmasının Tasarlanması</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Proje hata denetimi ve Proje Teslimi</t>
+    <t>Giriş Sahnesi  Ve Panellerin Tasarımı -  Oyun İçin Görsellerin Tasarımı Ve Ses Dosyalarının Eklenmsei</t>
   </si>
 </sst>
 </file>
@@ -205,9 +196,7 @@
             <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:effectLst>
                   <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
@@ -223,7 +212,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="tr-TR"/>
-              <a:t>Sahip Bulma Oyunu</a:t>
+              <a:t>Uçan Maymun</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -244,9 +233,7 @@
           <a:pPr>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:effectLst>
                 <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
@@ -328,17 +315,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="lt1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -378,9 +361,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sayfa1!$B$2:$B$8</c:f>
+              <c:f>Sayfa1!$B$2:$B$5</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Oyun İçin Gereksinimlerin Belirlenmesi</c:v>
                 </c:pt>
@@ -388,18 +371,9 @@
                   <c:v>Gereksinimlerin Değerlendirilmesi Ve Temel Mekanizmanın Tasarlanması</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Giriş Sahnesi  Ve Panellerin Tasarımı</c:v>
+                  <c:v>Giriş Sahnesi  Ve Panellerin Tasarımı -  Oyun İçin Görsellerin Tasarımı Ve Ses Dosyalarının Eklenmsei</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Oyun Mekanizmasının Yeni Sahneye Uyarlanması</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Oyun İçin Görsellerin Tasarımı Ve Ses Dosyalarının Eklenmsei</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Geri Sayım ve Puan Mekanizmasının Tasarlanması</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v> Proje hata denetimi ve Proje Teslimi</c:v>
                 </c:pt>
               </c:strCache>
@@ -407,30 +381,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sayfa1!$A$2:$A$8</c:f>
+              <c:f>Sayfa1!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>d/mm</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>45026</c:v>
+                  <c:v>45068</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45033</c:v>
+                  <c:v>45075</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45040</c:v>
+                  <c:v>45082</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45047</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45054</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45061</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45068</c:v>
+                  <c:v>45089</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -498,17 +463,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="lt1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -548,9 +509,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sayfa1!$B$2:$B$8</c:f>
+              <c:f>Sayfa1!$B$2:$B$5</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Oyun İçin Gereksinimlerin Belirlenmesi</c:v>
                 </c:pt>
@@ -558,18 +519,9 @@
                   <c:v>Gereksinimlerin Değerlendirilmesi Ve Temel Mekanizmanın Tasarlanması</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Giriş Sahnesi  Ve Panellerin Tasarımı</c:v>
+                  <c:v>Giriş Sahnesi  Ve Panellerin Tasarımı -  Oyun İçin Görsellerin Tasarımı Ve Ses Dosyalarının Eklenmsei</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Oyun Mekanizmasının Yeni Sahneye Uyarlanması</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Oyun İçin Görsellerin Tasarımı Ve Ses Dosyalarının Eklenmsei</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Geri Sayım ve Puan Mekanizmasının Tasarlanması</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v> Proje hata denetimi ve Proje Teslimi</c:v>
                 </c:pt>
               </c:strCache>
@@ -577,10 +529,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sayfa1!$C$2:$C$8</c:f>
+              <c:f>Sayfa1!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>7</c:v>
                 </c:pt>
@@ -591,15 +543,6 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
@@ -656,9 +599,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -714,9 +655,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -754,9 +693,7 @@
             <a:pPr rtl="0">
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -780,26 +717,9 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
+    <a:solidFill>
+      <a:schemeClr val="dk1"/>
+    </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -810,7 +730,14 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:latin typeface="+mn-lt"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="tr-TR"/>
     </a:p>
@@ -1626,7 +1553,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1649,7 +1576,7 @@
     </row>
     <row r="2" spans="1:3" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>45026</v>
+        <v>45068</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -1660,7 +1587,7 @@
     </row>
     <row r="3" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
-        <v>45033</v>
+        <v>45075</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
@@ -1669,12 +1596,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
-        <v>45040</v>
+        <v>45082</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>7</v>
@@ -1682,71 +1609,38 @@
     </row>
     <row r="5" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <v>45047</v>
+        <v>45089</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>45054</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>45061</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>45068</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="6" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B7" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+    <row r="8" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B8" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+    <row r="9" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="15" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>